<commit_message>
updated schedule management data
</commit_message>
<xml_diff>
--- a/Schedule Management.xlsx
+++ b/Schedule Management.xlsx
@@ -1,27 +1,153 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538360\Documents\github\GDP-1-project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E1688D3-A17B-4E37-9E8D-2BB2C647CD4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+  <si>
+    <t>Work Breakdown Structure Categories</t>
+  </si>
+  <si>
+    <t>Initiating</t>
+  </si>
+  <si>
+    <t>Planning</t>
+  </si>
+  <si>
+    <t>Designing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    UI Design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Synthesis of Design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Implementation Iteration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Early release and contract finalization</t>
+  </si>
+  <si>
+    <t>Implementation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Application Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    PWA Implementation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Android/IOS implementation</t>
+  </si>
+  <si>
+    <t>Monitoring and controlling</t>
+  </si>
+  <si>
+    <t>Closing</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Responsible</t>
+  </si>
+  <si>
+    <t>Estimated Hours per person</t>
+  </si>
+  <si>
+    <t>Sumana Reddy</t>
+  </si>
+  <si>
+    <t>Pooja</t>
+  </si>
+  <si>
+    <t>Vikas</t>
+  </si>
+  <si>
+    <t>Sumanth</t>
+  </si>
+  <si>
+    <t>Rajashekar</t>
+  </si>
+  <si>
+    <t>Rohith</t>
+  </si>
+  <si>
+    <t>Total Est.Hours</t>
+  </si>
+  <si>
+    <t>11/31/2020</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>Sumana</t>
+  </si>
+  <si>
+    <t>pooja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vikas </t>
+  </si>
+  <si>
+    <t>Rohit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                                                                    Schedule Management - Team : 01</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -37,7 +163,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +171,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +487,526 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="33.6328125" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" customWidth="1"/>
+    <col min="3" max="3" width="11.36328125" customWidth="1"/>
+    <col min="4" max="4" width="10.90625" customWidth="1"/>
+    <col min="5" max="5" width="24.54296875" customWidth="1"/>
+    <col min="9" max="9" width="9.453125" customWidth="1"/>
+    <col min="11" max="11" width="14.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="5">
+        <v>44065</v>
+      </c>
+      <c r="C7" s="6">
+        <v>44066</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="H7" s="2">
+        <v>2</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1</v>
+      </c>
+      <c r="J7" s="2">
+        <v>2</v>
+      </c>
+      <c r="K7" s="2">
+        <f>E7+F7+G7+H7+I7+J7</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="5">
+        <v>44066</v>
+      </c>
+      <c r="C8" s="6">
+        <v>44067</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="H8" s="2">
+        <v>2</v>
+      </c>
+      <c r="I8" s="2">
+        <v>2</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="K8" s="2">
+        <f>E8+F8+G8+H8+I8+J8</f>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="5">
+        <v>44068</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="F9" s="2">
+        <v>3</v>
+      </c>
+      <c r="G9" s="2">
+        <v>2</v>
+      </c>
+      <c r="H9" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="I9" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1</v>
+      </c>
+      <c r="K9" s="2">
+        <f>E9+F9+G9+H9+I9+J9</f>
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="5">
+        <v>44068</v>
+      </c>
+      <c r="C10" s="6">
+        <v>44089</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2">
+        <v>6</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2">
+        <f>F10</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="5">
+        <v>44090</v>
+      </c>
+      <c r="C11" s="6">
+        <v>44119</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="F11" s="2">
+        <v>2</v>
+      </c>
+      <c r="G11" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="J11" s="2">
+        <v>2</v>
+      </c>
+      <c r="K11" s="2">
+        <f>E11+F11+G11+H11+I11+J11</f>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="5">
+        <v>44120</v>
+      </c>
+      <c r="C12" s="5">
+        <v>44139</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2">
+        <f>G12</f>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="5">
+        <v>44140</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2">
+        <v>7</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2">
+        <f>I13</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="5">
+        <v>44216</v>
+      </c>
+      <c r="C14" s="5">
+        <v>44285</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2">
+        <v>2</v>
+      </c>
+      <c r="G14" s="2">
+        <v>3</v>
+      </c>
+      <c r="H14" s="2">
+        <v>2</v>
+      </c>
+      <c r="I14" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="J14" s="2">
+        <v>1</v>
+      </c>
+      <c r="K14" s="2">
+        <f>E14+F14+G14+H14+I14+J14</f>
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="5">
+        <v>44216</v>
+      </c>
+      <c r="C15" s="5">
+        <v>44232</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="2">
+        <v>2</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="G15" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="I15" s="2">
+        <v>2</v>
+      </c>
+      <c r="J15" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="K15" s="2">
+        <f>E15+F15+G15+H15+I15+J15</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="5">
+        <v>44233</v>
+      </c>
+      <c r="C16" s="5">
+        <v>44255</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="2">
+        <v>5</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2">
+        <f>E16</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="5">
+        <v>44256</v>
+      </c>
+      <c r="C17" s="5">
+        <v>44285</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2">
+        <v>6</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2">
+        <f>H17</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="5">
+        <v>44289</v>
+      </c>
+      <c r="C18" s="5">
+        <v>44303</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="G18" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="H18" s="2">
+        <v>4</v>
+      </c>
+      <c r="I18" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="J18" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="K18" s="2">
+        <f>E18+F18+G18+H18+I18+J18</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="5">
+        <v>44304</v>
+      </c>
+      <c r="C19" s="5">
+        <v>44317</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="K19" s="2">
+        <f>J19</f>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2">
+        <f>E7+E8+E9+E11+E14+E15+E16+E18</f>
+        <v>15</v>
+      </c>
+      <c r="F20" s="2">
+        <f>F7+F8+F9+F10+F11+F14+F15+F18</f>
+        <v>20</v>
+      </c>
+      <c r="G20" s="2">
+        <f>G7+G8+G9+G11+G12+G14+G15+G18</f>
+        <v>20</v>
+      </c>
+      <c r="H20" s="2">
+        <f>H7+H8+H9+H14+H15+H17+H18</f>
+        <v>20</v>
+      </c>
+      <c r="I20" s="2">
+        <f>I7+I8+I9+I11+I13+I14+I15+I18</f>
+        <v>18</v>
+      </c>
+      <c r="J20" s="2">
+        <f>J7+J8+J9+J11+J14+J15+J18+J19</f>
+        <v>17</v>
+      </c>
+      <c r="K20" s="2">
+        <f>K7+K8+K9+K10+K11+K12+K13+K14+K15+K16+K17+K18+K19</f>
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:XFD1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>